<commit_message>
Got his formula captured
</commit_message>
<xml_diff>
--- a/Power_Query_Challenge_165.xlsx
+++ b/Power_Query_Challenge_165.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE69F731-8241-4696-A38B-5F209674CD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FB711E-FBD0-4354-8834-79FE709896DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,6 +35,28 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
@@ -99,7 +121,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +136,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -288,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -308,6 +336,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,117 +490,18 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>60531</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>97790</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>5363</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>162560</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="A person in a red shirt and black jacket&#10;&#10;Description automatically generated">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE62AA26-CDC0-6CB5-7207-8C61F3D1811A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10682811" y="22860"/>
-          <a:ext cx="1773632" cy="6540500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>86360</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>109220</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>175681</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5" descr="A close-up of several logos&#10;&#10;Description automatically generated">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60C42E8A-BCB7-4985-AF99-8B51F2AC3342}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12537440" y="3035300"/>
-          <a:ext cx="1005840" cy="615101"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>560070</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>353060</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>125730</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>326390</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -584,7 +516,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6305550" y="1103630"/>
+          <a:off x="0" y="3755390"/>
           <a:ext cx="4060190" cy="2131060"/>
         </a:xfrm>
         <a:prstGeom prst="cloudCallout">
@@ -642,6 +574,50 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>17309</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95124</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C8D4034-EA14-88C1-B13D-3D57F151F132}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4914900" y="4206240"/>
+          <a:ext cx="13923809" cy="1009524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -910,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -924,10 +900,10 @@
     <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" customWidth="1"/>
+    <col min="9" max="9" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -949,8 +925,37 @@
       <c r="I1" s="16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K1" t="str" cm="1">
+        <f t="array" ref="K1:N15">_xlfn.LET(_xlpm.z,A2:C11,_xlpm.a,A2:A11,_xlpm.d,_xlfn.SCAN(,_xlpm.a,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,IF(_xlpm.v&gt;0,_xlpm.v,_xlpm.a))),_xlpm.e,_xlfn.DROP(_xlfn.VSTACK(_xlpm.d,0),1)&lt;&gt;_xlpm.d,
+_xlpm.v,_xlfn.VSTACK(_xlfn.REDUCE(A1:C1,_xlfn.SEQUENCE(ROWS(_xlpm.a)),_xlfn.LAMBDA(_xlpm.c,_xlpm.n,_xlfn.VSTACK(_xlpm.c,_xlfn.TAKE(_xlfn.VSTACK(_xlfn.HSTACK(INDEX(_xlpm.a&amp;"",_xlpm.n),_xlfn.DROP(INDEX(_xlpm.z,_xlpm.n,),,1)),
+_xlfn.HSTACK("Total",SUM(N(_xlfn.SINGLE(INDEX(_xlpm.d,_xlpm.n,1))=_xlpm.d)),SUM((_xlfn.DROP(_xlpm.z,,2)*(INDEX(_xlpm.d,_xlpm.n,1)=_xlpm.d))))),1+_xlfn.SINGLE(INDEX(_xlpm.e,_xlpm.n)))))),_xlfn.HSTACK("Grand Total",ROWS(_xlpm.d),SUM(_xlpm.z))),
+_xlfn.HSTACK(_xlpm.v,IFERROR(_xlfn.DROP(_xlpm.v,,2)/10,"Max Bonus")))</f>
+        <v>Dept</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Emp</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="N1" t="str">
+        <v>Max Bonus</v>
+      </c>
+      <c r="P1" t="b" cm="1">
+        <f t="array" ref="P1:S15">F1:I15=_xlfn.ANCHORARRAY(K1)</f>
+        <v>1</v>
+      </c>
+      <c r="Q1" t="b">
+        <v>1</v>
+      </c>
+      <c r="R1" t="b">
+        <v>1</v>
+      </c>
+      <c r="S1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -972,8 +977,32 @@
       <c r="I2" s="17">
         <v>19880</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K2" t="str">
+        <v>HR</v>
+      </c>
+      <c r="L2" t="str">
+        <v>Atkins</v>
+      </c>
+      <c r="M2">
+        <v>198800</v>
+      </c>
+      <c r="N2">
+        <v>19880</v>
+      </c>
+      <c r="P2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
         <v>6</v>
@@ -991,8 +1020,32 @@
       <c r="I3" s="17">
         <v>13360</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K3" t="str">
+        <v/>
+      </c>
+      <c r="L3" t="str">
+        <v>Warner</v>
+      </c>
+      <c r="M3">
+        <v>133600</v>
+      </c>
+      <c r="N3">
+        <v>13360</v>
+      </c>
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
         <v>7</v>
@@ -1010,8 +1063,32 @@
       <c r="I4" s="17">
         <v>17710</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K4" t="str">
+        <v/>
+      </c>
+      <c r="L4" t="str">
+        <v>Byrd</v>
+      </c>
+      <c r="M4">
+        <v>177100</v>
+      </c>
+      <c r="N4">
+        <v>17710</v>
+      </c>
+      <c r="P4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="b">
+        <v>1</v>
+      </c>
+      <c r="R4" t="b">
+        <v>1</v>
+      </c>
+      <c r="S4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1033,8 +1110,32 @@
       <c r="I5" s="17">
         <v>50950</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K5" t="str">
+        <v>Total</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <v>509500</v>
+      </c>
+      <c r="N5">
+        <v>50950</v>
+      </c>
+      <c r="P5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="b">
+        <v>1</v>
+      </c>
+      <c r="R5" t="b">
+        <v>1</v>
+      </c>
+      <c r="S5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="5" t="s">
         <v>11</v>
@@ -1054,8 +1155,32 @@
       <c r="I6" s="17">
         <v>16990</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K6" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="L6" t="str">
+        <v>Mccarty</v>
+      </c>
+      <c r="M6">
+        <v>169900</v>
+      </c>
+      <c r="N6">
+        <v>16990</v>
+      </c>
+      <c r="P6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="b">
+        <v>1</v>
+      </c>
+      <c r="R6" t="b">
+        <v>1</v>
+      </c>
+      <c r="S6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
         <v>12</v>
@@ -1073,8 +1198,32 @@
       <c r="I7" s="17">
         <v>10910</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K7" t="str">
+        <v/>
+      </c>
+      <c r="L7" t="str">
+        <v>Cooke</v>
+      </c>
+      <c r="M7">
+        <v>109100</v>
+      </c>
+      <c r="N7">
+        <v>10910</v>
+      </c>
+      <c r="P7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="b">
+        <v>1</v>
+      </c>
+      <c r="R7" t="b">
+        <v>1</v>
+      </c>
+      <c r="S7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
         <v>13</v>
@@ -1092,8 +1241,32 @@
       <c r="I8" s="17">
         <v>12250</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K8" t="str">
+        <v/>
+      </c>
+      <c r="L8" t="str">
+        <v>Johnson</v>
+      </c>
+      <c r="M8">
+        <v>122500</v>
+      </c>
+      <c r="N8">
+        <v>12250</v>
+      </c>
+      <c r="P8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="b">
+        <v>1</v>
+      </c>
+      <c r="R8" t="b">
+        <v>1</v>
+      </c>
+      <c r="S8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
         <v>14</v>
@@ -1111,8 +1284,32 @@
       <c r="I9" s="17">
         <v>8060</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K9" t="str">
+        <v/>
+      </c>
+      <c r="L9" t="str">
+        <v>Alexander</v>
+      </c>
+      <c r="M9">
+        <v>80600</v>
+      </c>
+      <c r="N9">
+        <v>8060</v>
+      </c>
+      <c r="P9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="b">
+        <v>1</v>
+      </c>
+      <c r="R9" t="b">
+        <v>1</v>
+      </c>
+      <c r="S9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
@@ -1132,8 +1329,32 @@
       <c r="I10" s="17">
         <v>10040</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K10" t="str">
+        <v/>
+      </c>
+      <c r="L10" t="str">
+        <v>Pierce</v>
+      </c>
+      <c r="M10">
+        <v>100400</v>
+      </c>
+      <c r="N10">
+        <v>10040</v>
+      </c>
+      <c r="P10" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q10" t="b">
+        <v>1</v>
+      </c>
+      <c r="R10" t="b">
+        <v>1</v>
+      </c>
+      <c r="S10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="8" t="s">
         <v>17</v>
@@ -1153,8 +1374,32 @@
       <c r="I11" s="17">
         <v>58250</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K11" t="str">
+        <v>Total</v>
+      </c>
+      <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="M11">
+        <v>582500</v>
+      </c>
+      <c r="N11">
+        <v>58250</v>
+      </c>
+      <c r="P11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="b">
+        <v>1</v>
+      </c>
+      <c r="R11" t="b">
+        <v>1</v>
+      </c>
+      <c r="S11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F12" s="10" t="s">
         <v>15</v>
       </c>
@@ -1167,8 +1412,32 @@
       <c r="I12" s="17">
         <v>16640</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K12" t="str">
+        <v>Purchasing</v>
+      </c>
+      <c r="L12" t="str">
+        <v>Bender</v>
+      </c>
+      <c r="M12">
+        <v>166400</v>
+      </c>
+      <c r="N12">
+        <v>16640</v>
+      </c>
+      <c r="P12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q12" t="b">
+        <v>1</v>
+      </c>
+      <c r="R12" t="b">
+        <v>1</v>
+      </c>
+      <c r="S12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F13" s="10"/>
       <c r="G13" s="11" t="s">
         <v>17</v>
@@ -1179,8 +1448,32 @@
       <c r="I13" s="17">
         <v>17170</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K13" t="str">
+        <v/>
+      </c>
+      <c r="L13" t="str">
+        <v>Blair</v>
+      </c>
+      <c r="M13">
+        <v>171700</v>
+      </c>
+      <c r="N13">
+        <v>17170</v>
+      </c>
+      <c r="P13" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="b">
+        <v>1</v>
+      </c>
+      <c r="R13" t="b">
+        <v>1</v>
+      </c>
+      <c r="S13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F14" s="10" t="s">
         <v>10</v>
       </c>
@@ -1193,8 +1486,32 @@
       <c r="I14" s="17">
         <v>33810</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K14" t="str">
+        <v>Total</v>
+      </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <v>338100</v>
+      </c>
+      <c r="N14">
+        <v>33810</v>
+      </c>
+      <c r="P14" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="b">
+        <v>1</v>
+      </c>
+      <c r="R14" t="b">
+        <v>1</v>
+      </c>
+      <c r="S14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F15" s="12" t="s">
         <v>18</v>
       </c>
@@ -1205,6 +1522,244 @@
         <v>1430100</v>
       </c>
       <c r="I15" s="18">
+        <v>143010</v>
+      </c>
+      <c r="K15" t="str">
+        <v>Grand Total</v>
+      </c>
+      <c r="L15">
+        <v>10</v>
+      </c>
+      <c r="M15">
+        <v>1430100</v>
+      </c>
+      <c r="N15">
+        <v>143010</v>
+      </c>
+      <c r="P15" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="b">
+        <v>1</v>
+      </c>
+      <c r="R15" t="b">
+        <v>1</v>
+      </c>
+      <c r="S15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="9:12" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I43" s="19" t="str" cm="1">
+        <f t="array" ref="I43:L57">_xlfn.LET(_xlpm.z,A2:C11,_xlpm.a,A2:A11,_xlpm.d,_xlfn.SCAN(,_xlpm.a,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,IF(_xlpm.v&gt;0,_xlpm.v,_xlpm.a))),_xlpm.e,_xlfn.DROP(_xlfn.VSTACK(_xlpm.d,0),1)&lt;&gt;_xlpm.d,
+_xlpm.v,_xlfn.VSTACK(_xlfn.REDUCE(A1:C1,_xlfn.SEQUENCE(ROWS(_xlpm.a)),_xlfn.LAMBDA(_xlpm.c,_xlpm.n,_xlfn.VSTACK(_xlpm.c,_xlfn.TAKE(_xlfn.VSTACK(_xlfn.HSTACK(INDEX(_xlpm.a&amp;"",_xlpm.n),_xlfn.DROP(INDEX(_xlpm.z,_xlpm.n,),,1)),
+_xlfn.HSTACK("Total",SUM(N(_xlfn.SINGLE(INDEX(_xlpm.d,_xlpm.n,1))=_xlpm.d)),SUM((_xlfn.DROP(_xlpm.z,,2)*(INDEX(_xlpm.d,_xlpm.n,1)=_xlpm.d))))),1+_xlfn.SINGLE(INDEX(_xlpm.e,_xlpm.n)))))),_xlfn.HSTACK("Grand Total",ROWS(_xlpm.d),SUM(_xlpm.z))),
+_xlfn.HSTACK(_xlpm.v,IFERROR(_xlfn.DROP(_xlpm.v,,2)/10,"Max Bonus")))</f>
+        <v>Dept</v>
+      </c>
+      <c r="J43" t="str">
+        <v>Emp</v>
+      </c>
+      <c r="K43" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="L43" t="str">
+        <v>Max Bonus</v>
+      </c>
+    </row>
+    <row r="44" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I44" t="str">
+        <v>HR</v>
+      </c>
+      <c r="J44" t="str">
+        <v>Atkins</v>
+      </c>
+      <c r="K44">
+        <v>198800</v>
+      </c>
+      <c r="L44">
+        <v>19880</v>
+      </c>
+    </row>
+    <row r="45" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I45" t="str">
+        <v/>
+      </c>
+      <c r="J45" t="str">
+        <v>Warner</v>
+      </c>
+      <c r="K45">
+        <v>133600</v>
+      </c>
+      <c r="L45">
+        <v>13360</v>
+      </c>
+    </row>
+    <row r="46" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I46" t="str">
+        <v/>
+      </c>
+      <c r="J46" t="str">
+        <v>Byrd</v>
+      </c>
+      <c r="K46">
+        <v>177100</v>
+      </c>
+      <c r="L46">
+        <v>17710</v>
+      </c>
+    </row>
+    <row r="47" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I47" t="str">
+        <v>Total</v>
+      </c>
+      <c r="J47">
+        <v>3</v>
+      </c>
+      <c r="K47">
+        <v>509500</v>
+      </c>
+      <c r="L47">
+        <v>50950</v>
+      </c>
+    </row>
+    <row r="48" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I48" t="str">
+        <v>Sales</v>
+      </c>
+      <c r="J48" t="str">
+        <v>Mccarty</v>
+      </c>
+      <c r="K48">
+        <v>169900</v>
+      </c>
+      <c r="L48">
+        <v>16990</v>
+      </c>
+    </row>
+    <row r="49" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I49" t="str">
+        <v/>
+      </c>
+      <c r="J49" t="str">
+        <v>Cooke</v>
+      </c>
+      <c r="K49">
+        <v>109100</v>
+      </c>
+      <c r="L49">
+        <v>10910</v>
+      </c>
+    </row>
+    <row r="50" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I50" t="str">
+        <v/>
+      </c>
+      <c r="J50" t="str">
+        <v>Johnson</v>
+      </c>
+      <c r="K50">
+        <v>122500</v>
+      </c>
+      <c r="L50">
+        <v>12250</v>
+      </c>
+    </row>
+    <row r="51" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I51" t="str">
+        <v/>
+      </c>
+      <c r="J51" t="str">
+        <v>Alexander</v>
+      </c>
+      <c r="K51">
+        <v>80600</v>
+      </c>
+      <c r="L51">
+        <v>8060</v>
+      </c>
+    </row>
+    <row r="52" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I52" t="str">
+        <v/>
+      </c>
+      <c r="J52" t="str">
+        <v>Pierce</v>
+      </c>
+      <c r="K52">
+        <v>100400</v>
+      </c>
+      <c r="L52">
+        <v>10040</v>
+      </c>
+    </row>
+    <row r="53" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I53" t="str">
+        <v>Total</v>
+      </c>
+      <c r="J53">
+        <v>5</v>
+      </c>
+      <c r="K53">
+        <v>582500</v>
+      </c>
+      <c r="L53">
+        <v>58250</v>
+      </c>
+    </row>
+    <row r="54" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I54" t="str">
+        <v>Purchasing</v>
+      </c>
+      <c r="J54" t="str">
+        <v>Bender</v>
+      </c>
+      <c r="K54">
+        <v>166400</v>
+      </c>
+      <c r="L54">
+        <v>16640</v>
+      </c>
+    </row>
+    <row r="55" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I55" t="str">
+        <v/>
+      </c>
+      <c r="J55" t="str">
+        <v>Blair</v>
+      </c>
+      <c r="K55">
+        <v>171700</v>
+      </c>
+      <c r="L55">
+        <v>17170</v>
+      </c>
+    </row>
+    <row r="56" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I56" t="str">
+        <v>Total</v>
+      </c>
+      <c r="J56">
+        <v>2</v>
+      </c>
+      <c r="K56">
+        <v>338100</v>
+      </c>
+      <c r="L56">
+        <v>33810</v>
+      </c>
+    </row>
+    <row r="57" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I57" t="str">
+        <v>Grand Total</v>
+      </c>
+      <c r="J57">
+        <v>10</v>
+      </c>
+      <c r="K57">
+        <v>1430100</v>
+      </c>
+      <c r="L57">
         <v>143010</v>
       </c>
     </row>

</xml_diff>